<commit_message>
First draggable test Data Drivem implemented
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
     <sheet name="DataSetRegistrationUser" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="DataSetInteractionPages" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$A$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataSetInteractionPages!$A$1:$A$31</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="98">
   <si>
     <t>Key</t>
   </si>
@@ -497,6 +497,15 @@
   </si>
   <si>
     <t>0,1</t>
+  </si>
+  <si>
+    <t>DefaultFunctionality_DragToOppositeCorner_ElementMovedToOppositeCorner</t>
+  </si>
+  <si>
+    <t>HorizontalOffset</t>
+  </si>
+  <si>
+    <t>VerticalOffset</t>
   </si>
 </sst>
 </file>
@@ -929,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
@@ -2329,14 +2338,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented Page scroll Up
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="99">
   <si>
     <t>Key</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>VerticalOffset</t>
+  </si>
+  <si>
+    <t>ConstrainMovementHorizontal_DragDiagonally_ElementMovedHorizontallyOnly</t>
   </si>
 </sst>
 </file>
@@ -2338,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2373,6 +2376,17 @@
         <v>140</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Selectable first test stuck
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="120">
   <si>
     <t>Key</t>
   </si>
@@ -616,6 +616,21 @@
   </si>
   <si>
     <t>ResizableConstrainedItem_ResizeSidesMoreThanConstraints_ItemResizeConstrainedByConstraints</t>
+  </si>
+  <si>
+    <t>SelectableItems_SelectThree_SelectedElementsStatusChangedToSelected</t>
+  </si>
+  <si>
+    <t>Selectable</t>
+  </si>
+  <si>
+    <t>Item 5</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>Item 1</t>
   </si>
 </sst>
 </file>
@@ -2464,10 +2479,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2619,6 +2634,23 @@
         <v>113</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
First selectable test ready, changed ItemCat? to Item?, Used list in selectableMap
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="117">
   <si>
     <t>Key</t>
   </si>
@@ -591,15 +591,6 @@
     <t>Droppable</t>
   </si>
   <si>
-    <t>ItemCat1</t>
-  </si>
-  <si>
-    <t>ItemCat2</t>
-  </si>
-  <si>
-    <t>ItemCat3</t>
-  </si>
-  <si>
     <t>Lolcat Shirt</t>
   </si>
   <si>
@@ -618,19 +609,19 @@
     <t>ResizableConstrainedItem_ResizeSidesMoreThanConstraints_ItemResizeConstrainedByConstraints</t>
   </si>
   <si>
-    <t>SelectableItems_SelectThree_SelectedElementsStatusChangedToSelected</t>
-  </si>
-  <si>
     <t>Selectable</t>
   </si>
   <si>
-    <t>Item 5</t>
-  </si>
-  <si>
-    <t>Item 2</t>
-  </si>
-  <si>
-    <t>Item 1</t>
+    <t>SelectableItems_SelectTwo_SelectedElementsStatusChangedToSelected</t>
+  </si>
+  <si>
+    <t>Item1</t>
+  </si>
+  <si>
+    <t>Item2</t>
+  </si>
+  <si>
+    <t>Item3</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
@@ -2479,10 +2470,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2506,13 +2497,13 @@
         <v>97</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9" t="s">
@@ -2523,12 +2514,15 @@
       <c r="A2" t="s">
         <v>95</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>150</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>140</v>
       </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="H2" t="s">
         <v>102</v>
       </c>
@@ -2537,12 +2531,15 @@
       <c r="A3" t="s">
         <v>98</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>15</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="H3" t="s">
         <v>102</v>
       </c>
@@ -2551,12 +2548,15 @@
       <c r="A4" t="s">
         <v>99</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>25</v>
       </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="H4" t="s">
         <v>102</v>
       </c>
@@ -2565,12 +2565,15 @@
       <c r="A5" t="s">
         <v>100</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>10</v>
       </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="H5" t="s">
         <v>102</v>
       </c>
@@ -2579,77 +2582,116 @@
       <c r="A6" t="s">
         <v>101</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>100</v>
       </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="H6" t="s">
         <v>102</v>
       </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>104</v>
       </c>
-      <c r="D8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" t="s">
-        <v>111</v>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H8" t="s">
         <v>105</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10">
+        <v>109</v>
+      </c>
+      <c r="B10" s="2">
         <v>120</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>90</v>
       </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11">
+        <v>111</v>
+      </c>
+      <c r="B11" s="2">
         <v>350</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>250</v>
       </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>113</v>
-      </c>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" t="s">
-        <v>117</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>116</v>
-      </c>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First sortable test ready
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="122">
   <si>
     <t>Key</t>
   </si>
@@ -628,6 +628,15 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>DefaultFunctionality_DragLastItemToListTop_LastItemIsAtListTop</t>
+  </si>
+  <si>
+    <t>Sortable</t>
+  </si>
+  <si>
+    <t>ConnectLists_DragOneSortableItemFromFirstListToSecondList_SortableItemItemMovedToSecondList</t>
   </si>
 </sst>
 </file>
@@ -2476,10 +2485,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2707,6 +2716,31 @@
         <v>112</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Sortable test 2 written
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="123">
   <si>
     <t>Key</t>
   </si>
@@ -636,7 +636,10 @@
     <t>Sortable</t>
   </si>
   <si>
-    <t>ConnectLists_DragOneSortableItemFromFirstListToSecondList_SortableItemItemMovedToSecondList</t>
+    <t>ConnectLists_DragOneSortableItemFromFirstListToSecondList_NumberOfItemsChangedAccordingly</t>
+  </si>
+  <si>
+    <t>Grid_DragOneSortableItemAfterAnother_OrderOfNumberedSortableItemsChangedAccordingly</t>
   </si>
 </sst>
 </file>
@@ -2485,10 +2488,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2734,11 +2737,22 @@
       <c r="A17" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="2">
-        <v>5</v>
+      <c r="D17" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="H17" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amend slightly Readme3.txt and UserData.xlsx
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="123">
   <si>
     <t>Key</t>
   </si>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2491,7 +2491,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2754,6 +2754,9 @@
       <c r="E18" s="2">
         <v>7</v>
       </c>
+      <c r="H18" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reformat (some of) RegistrationUser Tests to use unified method GetData and FIllIn
</commit_message>
<xml_diff>
--- a/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
+++ b/SeleniumTestsDemoQaPage/DataDrivenTests/UserData.xlsx
@@ -225,7 +225,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>vankatabe:</t>
         </r>
@@ -234,7 +235,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 size constraint</t>
@@ -249,7 +251,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">vankatabe:
 </t>
@@ -271,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="125">
   <si>
     <t>Key</t>
   </si>
@@ -504,9 +507,6 @@
     <t>* Fields do not match</t>
   </si>
   <si>
-    <t>effect</t>
-  </si>
-  <si>
     <t>username + email</t>
   </si>
   <si>
@@ -640,13 +640,22 @@
   </si>
   <si>
     <t>Grid_DragOneSortableItemAfterAnother_OrderOfNumberedSortableItemsChangedAccordingly</t>
+  </si>
+  <si>
+    <t>Asserter</t>
+  </si>
+  <si>
+    <t>AssertNameErrorMessage</t>
+  </si>
+  <si>
+    <t>Effect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,19 +694,6 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1086,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1113,11 +1109,12 @@
     <col min="17" max="17" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.7265625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="2"/>
+    <col min="20" max="20" width="15.81640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="27.7265625" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
@@ -1175,11 +1172,14 @@
       <c r="S1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>21</v>
@@ -1235,11 +1235,14 @@
       <c r="S2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="U2" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>46</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>21</v>
@@ -1295,11 +1298,14 @@
       <c r="S3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>46</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>21</v>
@@ -1353,11 +1359,11 @@
       <c r="S4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="U4" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1413,11 +1419,11 @@
       <c r="S5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1440,7 +1446,7 @@
         <v>46</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>21</v>
@@ -1473,11 +1479,11 @@
       <c r="S6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="U6" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>46</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>21</v>
@@ -1535,11 +1541,11 @@
       <c r="S7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="U7" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1562,7 +1568,7 @@
         <v>46</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>21</v>
@@ -1597,11 +1603,11 @@
       <c r="S8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="U8" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1624,7 +1630,7 @@
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>21</v>
@@ -1657,11 +1663,11 @@
       <c r="S9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="6" t="s">
+      <c r="U9" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>46</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>21</v>
@@ -1719,11 +1725,11 @@
       <c r="S10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="U10" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>46</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>21</v>
@@ -1779,11 +1785,11 @@
       <c r="S11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="U11" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1806,7 +1812,7 @@
         <v>46</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>21</v>
@@ -1841,11 +1847,11 @@
       <c r="S12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T12" s="6" t="s">
+      <c r="U12" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1868,7 +1874,7 @@
         <v>46</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>21</v>
@@ -1903,11 +1909,11 @@
       <c r="S13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="U13" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>46</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>21</v>
@@ -1965,11 +1971,11 @@
       <c r="S14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T14" s="6" t="s">
+      <c r="U14" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1980,7 +1986,7 @@
         <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>20</v>
@@ -1992,7 +1998,7 @@
         <v>46</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>21</v>
@@ -2010,7 +2016,7 @@
         <v>27</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>23</v>
@@ -2027,11 +2033,11 @@
       <c r="S15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T15" s="6" t="s">
+      <c r="U15" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>61</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>20</v>
@@ -2054,7 +2060,7 @@
         <v>46</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>21</v>
@@ -2078,7 +2084,7 @@
         <v>23</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>25</v>
@@ -2089,11 +2095,11 @@
       <c r="S16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="6" t="s">
+      <c r="U16" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>17</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>20</v>
@@ -2116,7 +2122,7 @@
         <v>46</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>21</v>
@@ -2149,11 +2155,11 @@
       <c r="S17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="U17" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>18</v>
       </c>
@@ -2164,7 +2170,7 @@
         <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>20</v>
@@ -2176,7 +2182,7 @@
         <v>46</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>21</v>
@@ -2206,16 +2212,16 @@
         <v>25</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="U18" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>19</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>20</v>
@@ -2238,7 +2244,7 @@
         <v>46</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>21</v>
@@ -2271,11 +2277,12 @@
         <v>26</v>
       </c>
       <c r="S19" s="3"/>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="3"/>
+      <c r="U19" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>20</v>
       </c>
@@ -2286,7 +2293,7 @@
         <v>63</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>20</v>
@@ -2298,7 +2305,7 @@
         <v>46</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>21</v>
@@ -2331,13 +2338,14 @@
         <v>26</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="T20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="T20" s="3"/>
+      <c r="U20" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>21</v>
       </c>
@@ -2348,7 +2356,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>20</v>
@@ -2360,7 +2368,7 @@
         <v>46</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>21</v>
@@ -2393,24 +2401,25 @@
         <v>26</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="T21" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="T21" s="3"/>
+      <c r="U21" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>20</v>
@@ -2422,7 +2431,7 @@
         <v>46</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>21</v>
@@ -2457,21 +2466,21 @@
       <c r="S22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T22" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U22" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2509,28 +2518,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>97</v>
-      </c>
       <c r="D1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="2">
         <v>150</v>
@@ -2542,12 +2551,12 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -2559,12 +2568,12 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2">
         <v>20</v>
@@ -2576,12 +2585,12 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -2593,12 +2602,12 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2610,7 +2619,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2622,21 +2631,21 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="H8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2648,7 +2657,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="2">
         <v>120</v>
@@ -2660,12 +2669,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="2">
         <v>350</v>
@@ -2677,7 +2686,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -2689,7 +2698,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2701,27 +2710,27 @@
       </c>
       <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="H14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -2730,23 +2739,23 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -2755,7 +2764,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>